<commit_message>
sensor data modeled in IOF-Core and SAREF and align
</commit_message>
<xml_diff>
--- a/sensor-tank.xlsx
+++ b/sensor-tank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arkop\Nextcloud\Documents\OntoCommons\Stuttgart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arkop\git\oc-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5515B49-C6E3-4BD9-B82D-4CDBCF3C3F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9D0C12-9659-4913-9B0F-6DCD6C31C597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
   <si>
     <t xml:space="preserve">Sensor </t>
   </si>
@@ -117,6 +117,42 @@
   </si>
   <si>
     <t>Measurement</t>
+  </si>
+  <si>
+    <t>2022-11-03T09:22:08Z</t>
+  </si>
+  <si>
+    <t>2022-11-03T09:25:38Z</t>
+  </si>
+  <si>
+    <t>2022-11-03T09:29:08Z</t>
+  </si>
+  <si>
+    <t>2022-11-03T09:32:38Z</t>
+  </si>
+  <si>
+    <t>2022-11-03T09:36:08Z</t>
+  </si>
+  <si>
+    <t>2022-11-03T09:39:38Z</t>
+  </si>
+  <si>
+    <t>2022-11-06T17:31:51Z</t>
+  </si>
+  <si>
+    <t>2022-11-06T17:35:21Z</t>
+  </si>
+  <si>
+    <t>2022-11-06T17:38:51Z</t>
+  </si>
+  <si>
+    <t>2022-11-06T17:42:21Z</t>
+  </si>
+  <si>
+    <t>2022-11-06T17:45:51Z</t>
+  </si>
+  <si>
+    <t>2022-11-06T17:49:21Z</t>
   </si>
 </sst>
 </file>
@@ -125,7 +161,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy&quot; &quot;h:mm:ss&quot; &quot;AM/PM;@"/>
-    <numFmt numFmtId="167" formatCode="[$]hh:mm:ss;@" x16r2:formatCode16="[$-en-150,1]hh:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="[$]hh:mm:ss;@" x16r2:formatCode16="[$-en-150,1]hh:mm:ss;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -204,10 +240,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,7 +511,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C7" ca="1" si="0">RAND()*(25-20)+20</f>
-        <v>21.419430961925549</v>
+        <v>20.617588525741265</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -489,7 +525,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>23.590926391794817</v>
+        <v>23.575585055305172</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -503,7 +539,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>23.843858226494042</v>
+        <v>20.780583390109388</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -517,7 +553,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>20.852317420209982</v>
+        <v>20.320570234493584</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -531,7 +567,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>24.876757348785603</v>
+        <v>20.188568001500968</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -545,7 +581,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>21.622102983486339</v>
+        <v>21.018370634872142</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -555,12 +591,12 @@
       </c>
       <c r="B8" s="1">
         <f ca="1">NOW()</f>
-        <v>44871.738813888885</v>
+        <v>44983.559961226849</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
         <f t="shared" ref="D8:D19" ca="1" si="2">RAND()*(195-190)+190</f>
-        <v>193.31280045513236</v>
+        <v>194.76232315893566</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -569,12 +605,12 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ref="B9:B10" ca="1" si="3">B8+210/86400</f>
-        <v>44871.741244444442</v>
+        <v>44983.562391782405</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>194.91750018708279</v>
+        <v>190.67113846500231</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -583,12 +619,12 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>44871.743674999998</v>
+        <v>44983.564822337961</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>193.17938451981388</v>
+        <v>194.43377673564609</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -597,12 +633,12 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ref="B11:B13" ca="1" si="4">B10+210/86400</f>
-        <v>44871.746105555554</v>
+        <v>44983.567252893517</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>191.75352786360375</v>
+        <v>193.9354806162369</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -611,7 +647,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44871.74853611111</v>
+        <v>44983.569683449074</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
@@ -624,12 +660,12 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="4"/>
-        <v>44871.750966666666</v>
+        <v>44983.57211400463</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>193.29055028991502</v>
+        <v>192.42760438957063</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -638,12 +674,12 @@
       </c>
       <c r="B14" s="1">
         <f ca="1">NOW()</f>
-        <v>44871.738813888885</v>
+        <v>44983.559961226849</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>193.20821594696969</v>
+        <v>192.17147429854819</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -652,12 +688,12 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ref="B15:B19" ca="1" si="5">B14+210/86400</f>
-        <v>44871.741244444442</v>
+        <v>44983.562391782405</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>190.5377750851269</v>
+        <v>193.84024856122849</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -666,12 +702,12 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>44871.743674999998</v>
+        <v>44983.564822337961</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>191.55350173694259</v>
+        <v>192.15445418106771</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -680,12 +716,12 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>44871.746105555554</v>
+        <v>44983.567252893517</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>194.0380328883231</v>
+        <v>194.00379481735783</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -694,12 +730,12 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>44871.74853611111</v>
+        <v>44983.569683449074</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
         <f ca="1">RAND()*(195-190)+190</f>
-        <v>194.39579658142975</v>
+        <v>190.0592517624531</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -708,12 +744,12 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="5"/>
-        <v>44871.750966666666</v>
+        <v>44983.57211400463</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>192.24340638372954</v>
+        <v>190.21536026369367</v>
       </c>
     </row>
   </sheetData>
@@ -727,13 +763,13 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -756,8 +792,8 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
-        <v>44868.390370370369</v>
+      <c r="B2" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="2">
         <v>20.030458361315432</v>
@@ -768,8 +804,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
-        <v>44868.392800925925</v>
+      <c r="B3" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="2">
         <v>21.004742332331585</v>
@@ -780,8 +816,8 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
-        <v>44868.395231481481</v>
+      <c r="B4" t="s">
+        <v>29</v>
       </c>
       <c r="C4" s="2">
         <v>20.920434744180351</v>
@@ -792,8 +828,8 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
-        <v>44868.397662037038</v>
+      <c r="B5" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="2">
         <v>20.396641431702474</v>
@@ -804,8 +840,8 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>44868.400092592594</v>
+      <c r="B6" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="2">
         <v>20.314201216375029</v>
@@ -816,8 +852,8 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
-        <v>44868.40252314815</v>
+      <c r="B7" t="s">
+        <v>32</v>
       </c>
       <c r="C7" s="2">
         <v>21.972002583633241</v>
@@ -828,8 +864,8 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
-        <v>44871.730450810188</v>
+      <c r="B8" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
@@ -840,8 +876,8 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4">
-        <v>44871.732881365744</v>
+      <c r="B9" t="s">
+        <v>34</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
@@ -852,8 +888,8 @@
       <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4">
-        <v>44871.7353119213</v>
+      <c r="B10" t="s">
+        <v>35</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
@@ -864,8 +900,8 @@
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="4">
-        <v>44871.737742476857</v>
+      <c r="B11" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
@@ -876,8 +912,8 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4">
-        <v>44871.740173611113</v>
+      <c r="B12" t="s">
+        <v>37</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
@@ -888,8 +924,8 @@
       <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4">
-        <v>44871.742603587969</v>
+      <c r="B13" t="s">
+        <v>38</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2">
@@ -900,8 +936,8 @@
       <c r="A14" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4">
-        <v>44871.730450810188</v>
+      <c r="B14" t="s">
+        <v>33</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
@@ -912,8 +948,8 @@
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4">
-        <v>44871.732881365744</v>
+      <c r="B15" t="s">
+        <v>34</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2">
@@ -924,8 +960,8 @@
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="4">
-        <v>44871.7353119213</v>
+      <c r="B16" t="s">
+        <v>35</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2">
@@ -936,8 +972,8 @@
       <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="4">
-        <v>44871.737742476857</v>
+      <c r="B17" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2">
@@ -948,8 +984,8 @@
       <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="4">
-        <v>44871.740173032413</v>
+      <c r="B18" t="s">
+        <v>37</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2">
@@ -960,8 +996,8 @@
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="4">
-        <v>44871.742603587969</v>
+      <c r="B19" t="s">
+        <v>38</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2">
@@ -970,6 +1006,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>